<commit_message>
Added auto pronunciation for Recite
</commit_message>
<xml_diff>
--- a/软件功能开发进度列表.xlsx
+++ b/软件功能开发进度列表.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7230"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7230" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="change list" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="76">
   <si>
     <t>基础平台</t>
   </si>
@@ -235,6 +235,15 @@
   </si>
   <si>
     <t>下载文件到手机内存</t>
+  </si>
+  <si>
+    <t>public void writeBoolean(boolean val)</t>
+  </si>
+  <si>
+    <t>Added method</t>
+  </si>
+  <si>
+    <t>IFileOutputStream.java</t>
   </si>
 </sst>
 </file>
@@ -695,7 +704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
@@ -1415,12 +1424,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="C2:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6">
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>